<commit_message>
stage 4: edited statistical analysis and sampling
</commit_message>
<xml_diff>
--- a/Examples/descStats.xlsx
+++ b/Examples/descStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lr38/Desktop/masters-handbook/Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979C56C9-EEDD-4045-9446-6BA639313E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3F18A6-D7D8-5540-8702-F75767A1A717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21380" yWindow="3220" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{27B1E98A-9D20-C444-A7E5-83EBCA5C2C3E}"/>
+    <workbookView xWindow="21480" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{27B1E98A-9D20-C444-A7E5-83EBCA5C2C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,6 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1:$A$15</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$1:$A$15</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$1:$A$15</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -153,12 +151,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
@@ -183,7 +180,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1157,116 +1154,112 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>128.46666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>2.2079222438574768</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>8.5512460801809187</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>73.123809523809541</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>3.2279252485945813</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>-1.4163429834169987</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>1927</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>15</v>
       </c>
     </row>

</xml_diff>